<commit_message>
Other two sanity checks implemented
</commit_message>
<xml_diff>
--- a/data_v2.xlsx
+++ b/data_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alissa Vermast\PycharmProjects\technologiesForLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC9ABB5-30A9-414A-BE34-C9E2B3066C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6D23B4-BDB6-4FA3-9B3E-BBC52B62BAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6702" uniqueCount="5436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6703" uniqueCount="5436">
   <si>
     <t>Grade2</t>
   </si>
@@ -18785,18 +18785,21 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="63.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" customWidth="1"/>
     <col min="2" max="9" width="6.6640625" customWidth="1"/>
     <col min="10" max="10" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="57" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5379</v>
+      </c>
       <c r="B1" s="6" t="s">
         <v>5380</v>
       </c>
@@ -64050,18 +64053,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64083,18 +64086,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C43C01-44AE-4FFD-8FD0-70D69151138C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEA090E0-96EB-4C08-BCA9-FD24468CD521}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C43C01-44AE-4FFD-8FD0-70D69151138C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>